<commit_message>
Tried a bubble sort.
</commit_message>
<xml_diff>
--- a/topics.xlsx
+++ b/topics.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="86">
   <si>
     <t>Interview Prep</t>
   </si>
@@ -271,6 +271,15 @@
   </si>
   <si>
     <t>Big-O</t>
+  </si>
+  <si>
+    <t>Must keep the order; remember to include all methods (index, search, size, etc.)</t>
+  </si>
+  <si>
+    <t>n^2</t>
+  </si>
+  <si>
+    <t>Extremely slow, worst of the sorts, but fine for almost-sorted lists; easiest implementation for small lists too</t>
   </si>
 </sst>
 </file>
@@ -848,7 +857,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomRight" activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1882,8 +1891,8 @@
       <c r="E31">
         <v>3</v>
       </c>
-      <c r="J31" t="s">
-        <v>62</v>
+      <c r="J31">
+        <v>4</v>
       </c>
       <c r="K31" t="s">
         <v>62</v>
@@ -1952,8 +1961,11 @@
       <c r="E33">
         <v>3</v>
       </c>
-      <c r="J33" t="s">
-        <v>62</v>
+      <c r="H33" t="s">
+        <v>83</v>
+      </c>
+      <c r="J33">
+        <v>4</v>
       </c>
       <c r="K33" t="s">
         <v>63</v>
@@ -1984,8 +1996,17 @@
       <c r="E34">
         <v>3</v>
       </c>
-      <c r="J34" t="s">
-        <v>62</v>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>84</v>
+      </c>
+      <c r="H34" t="s">
+        <v>85</v>
+      </c>
+      <c r="J34">
+        <v>4</v>
       </c>
       <c r="K34" t="s">
         <v>63</v>

</xml_diff>

<commit_message>
Did some warmup problems.
</commit_message>
<xml_diff>
--- a/topics.xlsx
+++ b/topics.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="106">
   <si>
     <t>Interview Prep</t>
   </si>
@@ -331,6 +331,15 @@
   </si>
   <si>
     <t>Suffix Tree</t>
+  </si>
+  <si>
+    <t>O(nk) where k is the length of the longest number</t>
+  </si>
+  <si>
+    <t>Can only use with integers</t>
+  </si>
+  <si>
+    <t>O(k + n)</t>
   </si>
 </sst>
 </file>
@@ -379,7 +388,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="131">
+  <cellStyleXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -464,6 +473,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -516,7 +526,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="83"/>
   </cellXfs>
-  <cellStyles count="131">
+  <cellStyles count="132">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -605,6 +615,7 @@
     <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -982,7 +993,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L25" sqref="L25"/>
+      <selection pane="bottomRight" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1094,7 +1105,7 @@
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="M3" t="s">
         <v>60</v>
@@ -1135,10 +1146,10 @@
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>60</v>
-      </c>
-      <c r="M4" t="s">
-        <v>60</v>
+        <v>66</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
       </c>
       <c r="N4" t="s">
         <v>60</v>
@@ -1176,10 +1187,10 @@
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>60</v>
-      </c>
-      <c r="M5" t="s">
-        <v>60</v>
+        <v>66</v>
+      </c>
+      <c r="M5">
+        <v>2</v>
       </c>
       <c r="N5" t="s">
         <v>60</v>
@@ -1214,7 +1225,7 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M6" t="s">
         <v>64</v>
@@ -1255,7 +1266,7 @@
         <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="M7" t="s">
         <v>64</v>
@@ -1325,7 +1336,7 @@
         <v>66</v>
       </c>
       <c r="L9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M9" t="s">
         <v>65</v>
@@ -1360,7 +1371,7 @@
         <v>66</v>
       </c>
       <c r="L10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M10" t="s">
         <v>65</v>
@@ -1395,7 +1406,7 @@
         <v>2</v>
       </c>
       <c r="L11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M11" t="s">
         <v>65</v>
@@ -1471,7 +1482,7 @@
         <v>3</v>
       </c>
       <c r="L13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M13" t="s">
         <v>65</v>
@@ -1518,7 +1529,7 @@
         <v>3</v>
       </c>
       <c r="L14" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M14" t="s">
         <v>65</v>
@@ -1553,7 +1564,7 @@
         <v>2</v>
       </c>
       <c r="L15" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M15" t="s">
         <v>63</v>
@@ -1588,7 +1599,7 @@
         <v>66</v>
       </c>
       <c r="L16" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M16" t="s">
         <v>63</v>
@@ -1705,7 +1716,7 @@
         <v>4</v>
       </c>
       <c r="L19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="M19" t="s">
         <v>63</v>
@@ -1781,7 +1792,7 @@
         <v>2</v>
       </c>
       <c r="L21" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="M21" t="s">
         <v>59</v>
@@ -1816,7 +1827,7 @@
         <v>66</v>
       </c>
       <c r="L22" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="M22" t="s">
         <v>59</v>
@@ -1895,7 +1906,7 @@
         <v>4</v>
       </c>
       <c r="L24" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="M24" t="s">
         <v>59</v>
@@ -1939,7 +1950,7 @@
         <v>3</v>
       </c>
       <c r="L25" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="M25" t="s">
         <v>59</v>
@@ -1983,7 +1994,7 @@
         <v>4</v>
       </c>
       <c r="L26" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="M26" t="s">
         <v>59</v>
@@ -2018,7 +2029,7 @@
         <v>66</v>
       </c>
       <c r="L27" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="M27" t="s">
         <v>61</v>
@@ -2053,7 +2064,7 @@
         <v>2</v>
       </c>
       <c r="L28" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="M28" t="s">
         <v>61</v>
@@ -2088,7 +2099,7 @@
         <v>3</v>
       </c>
       <c r="L29" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="M29" t="s">
         <v>61</v>
@@ -2129,7 +2140,7 @@
         <v>3</v>
       </c>
       <c r="L30" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="M30" t="s">
         <v>61</v>
@@ -2170,7 +2181,7 @@
         <v>4</v>
       </c>
       <c r="L31" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="M31" t="s">
         <v>61</v>
@@ -2214,7 +2225,7 @@
         <v>4</v>
       </c>
       <c r="L32" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="M32" t="s">
         <v>61</v>
@@ -2249,7 +2260,7 @@
         <v>66</v>
       </c>
       <c r="L33" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="M33" t="s">
         <v>62</v>
@@ -2277,6 +2288,15 @@
       <c r="E34">
         <v>2</v>
       </c>
+      <c r="F34" t="s">
+        <v>105</v>
+      </c>
+      <c r="G34" t="s">
+        <v>103</v>
+      </c>
+      <c r="H34" t="s">
+        <v>104</v>
+      </c>
       <c r="J34" t="s">
         <v>66</v>
       </c>
@@ -2284,7 +2304,7 @@
         <v>66</v>
       </c>
       <c r="L34" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="M34" t="s">
         <v>62</v>
@@ -2319,7 +2339,7 @@
         <v>2</v>
       </c>
       <c r="L35" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="M35" t="s">
         <v>62</v>
@@ -2366,7 +2386,7 @@
         <v>3</v>
       </c>
       <c r="L36" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="M36" t="s">
         <v>62</v>
@@ -2401,7 +2421,7 @@
         <v>4</v>
       </c>
       <c r="L37" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="M37" t="s">
         <v>62</v>
@@ -2427,7 +2447,7 @@
         <v>66</v>
       </c>
       <c r="L38" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="M38" t="s">
         <v>62</v>
@@ -2453,7 +2473,7 @@
         <v>66</v>
       </c>
       <c r="L39" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="M39" t="s">
         <v>62</v>

</xml_diff>